<commit_message>
Printing of best dimensions
</commit_message>
<xml_diff>
--- a/RoundBar_Export.xlsx
+++ b/RoundBar_Export.xlsx
@@ -83,7 +83,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -111,11 +111,22 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
@@ -138,6 +149,17 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>